<commit_message>
Added change for final feedback
</commit_message>
<xml_diff>
--- a/frontend/src/assets/excel/Example Squad List.xlsx
+++ b/frontend/src/assets/excel/Example Squad List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zahoor/Desktop/Football data/The Football Project - Example Squad Sheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zahoor/Documents/docker/mean-docker_old/frontend/src/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F8515B-9B1B-A64A-86A0-3444FFB8016C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE237AD-200B-C247-AB08-B072C8967934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" xr2:uid="{F8A83BFD-9C1C-9D4D-BE21-DA336318B9E2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{F8A83BFD-9C1C-9D4D-BE21-DA336318B9E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="97">
   <si>
     <t>First Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>League</t>
   </si>
   <si>
-    <t>Player ID Number</t>
-  </si>
-  <si>
     <t>Wade</t>
   </si>
   <si>
@@ -149,57 +146,6 @@
     <t>ROSS</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>0009</t>
-  </si>
-  <si>
-    <t>0010</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
-    <t>0012</t>
-  </si>
-  <si>
-    <t>0013</t>
-  </si>
-  <si>
-    <t>0014</t>
-  </si>
-  <si>
-    <t>0015</t>
-  </si>
-  <si>
-    <t>0016</t>
-  </si>
-  <si>
-    <t>0017</t>
-  </si>
-  <si>
     <t>EID Front Upload</t>
   </si>
   <si>
@@ -290,55 +236,28 @@
     <t>786-1989-1234567-18</t>
   </si>
   <si>
-    <t>0018</t>
-  </si>
-  <si>
     <t>786-1989-1234567-19</t>
   </si>
   <si>
-    <t>0019</t>
-  </si>
-  <si>
     <t>786-1989-1234567-20</t>
   </si>
   <si>
-    <t>0020</t>
-  </si>
-  <si>
     <t>786-1989-1234567-21</t>
   </si>
   <si>
-    <t>0021</t>
-  </si>
-  <si>
     <t>786-1989-1234567-22</t>
   </si>
   <si>
-    <t>0022</t>
-  </si>
-  <si>
     <t>786-1989-1234567-23</t>
   </si>
   <si>
-    <t>0023</t>
-  </si>
-  <si>
     <t>786-1989-1234567-24</t>
   </si>
   <si>
-    <t>0024</t>
-  </si>
-  <si>
     <t>786-1989-1234567-25</t>
   </si>
   <si>
-    <t>0025</t>
-  </si>
-  <si>
     <t>786-1989-1234567-26</t>
-  </si>
-  <si>
-    <t>0026</t>
   </si>
   <si>
     <t>WALKER1</t>
@@ -809,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17709A5B-7574-F349-9EA2-2726CF5A96DD}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:F27"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -825,12 +744,11 @@
     <col min="6" max="6" width="30.5" customWidth="1"/>
     <col min="7" max="7" width="40.5" customWidth="1"/>
     <col min="8" max="8" width="39.1640625" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" customWidth="1"/>
-    <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="30.1640625" customWidth="1"/>
+    <col min="9" max="9" width="41" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
+    <row r="1" spans="1:11" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -844,33 +762,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="24">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5">
         <v>42252</v>
@@ -879,33 +794,30 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="24">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5">
         <v>42253</v>
@@ -914,34 +826,31 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="24">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5">
         <v>42254</v>
@@ -950,34 +859,31 @@
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="24">
+      <c r="J4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="24">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5">
         <v>42255</v>
@@ -986,34 +892,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="24">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5">
         <v>42256</v>
@@ -1022,34 +925,31 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="24">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5">
         <v>42257</v>
@@ -1058,34 +958,31 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="24">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5">
         <v>42258</v>
@@ -1094,34 +991,31 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="24">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5">
         <v>42259</v>
@@ -1130,34 +1024,31 @@
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="24">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5">
         <v>42260</v>
@@ -1166,34 +1057,31 @@
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="24">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5">
         <v>42261</v>
@@ -1202,34 +1090,31 @@
         <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="24">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5">
         <v>42262</v>
@@ -1238,34 +1123,31 @@
         <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="24">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5">
         <v>42263</v>
@@ -1274,34 +1156,31 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="24">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5">
         <v>42264</v>
@@ -1310,34 +1189,31 @@
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" ht="24">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5">
         <v>42265</v>
@@ -1346,34 +1222,31 @@
         <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" ht="24">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5">
         <v>42266</v>
@@ -1382,34 +1255,31 @@
         <v>15</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" ht="24">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="5">
         <v>42267</v>
@@ -1418,34 +1288,31 @@
         <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" ht="24">
+      <c r="A18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" ht="24">
-      <c r="A18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="C18" s="5">
         <v>42268</v>
@@ -1454,33 +1321,30 @@
         <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="24">
+      <c r="A19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="24">
-      <c r="A19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="C19" s="5">
         <v>42269</v>
@@ -1489,33 +1353,30 @@
         <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="24">
+      <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="24">
-      <c r="A20" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C20" s="5">
         <v>42270</v>
@@ -1524,33 +1385,30 @@
         <v>19</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="24">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5">
         <v>42271</v>
@@ -1559,33 +1417,30 @@
         <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="I21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24">
+      <c r="A22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="24">
-      <c r="A22" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="B22" s="4" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="C22" s="5">
         <v>42272</v>
@@ -1594,33 +1449,30 @@
         <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="24">
+      <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="24">
-      <c r="A23" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="B23" s="4" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5">
         <v>42273</v>
@@ -1629,33 +1481,30 @@
         <v>22</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="24">
       <c r="A24" s="3" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="C24" s="5">
         <v>42274</v>
@@ -1664,33 +1513,30 @@
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="24">
       <c r="A25" s="3" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="C25" s="5">
         <v>42275</v>
@@ -1699,33 +1545,30 @@
         <v>24</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="24">
       <c r="A26" s="3" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="C26" s="5">
         <v>42276</v>
@@ -1734,33 +1577,30 @@
         <v>25</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="24">
+        <v>40</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="24">
       <c r="A27" s="3" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C27" s="5">
         <v>42277</v>
@@ -1769,25 +1609,22 @@
         <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>57</v>
+        <v>40</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>